<commit_message>
Calculo das taxas e saida em txt completos
</commit_message>
<xml_diff>
--- a/dados/ARQUIVO PARA LER.xlsx
+++ b/dados/ARQUIVO PARA LER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ginfo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ginfo\eclipse-workspace\TesteVinicius\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4876918D-ED5A-4820-824C-84C40B46C212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100E3311-6CC8-41EA-A836-E8177445EC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-840" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FupContasReceber-27" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FupContasReceber-27'!$A$1:$O$935</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8391" uniqueCount="3600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8392" uniqueCount="3601">
   <si>
     <t>Nr Titulo</t>
   </si>
@@ -10833,12 +10823,15 @@
   </si>
   <si>
     <t>1558.000 - LCA CONSULTORES S.S.</t>
+  </si>
+  <si>
+    <t>464.52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11612,11 +11605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A913" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11724,8 +11717,8 @@
       <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="N2">
-        <v>464.52</v>
+      <c r="N2" t="s">
+        <v>3600</v>
       </c>
       <c r="O2" t="s">
         <v>23</v>
@@ -55493,7 +55486,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O935"/>
+  <autoFilter ref="A1:O935" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>